<commit_message>
Google Drive Base64 ortam değişkeni ile entegre edildi
</commit_message>
<xml_diff>
--- a/backend/backend/OneDrive_lojistik.xlsx
+++ b/backend/backend/OneDrive_lojistik.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,6 +653,556 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>31.03.2026</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>14</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>31.03.2026</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>14</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>9</v>
+      </c>
+      <c r="M6" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>09.10.1998</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>14</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>9</v>
+      </c>
+      <c r="M7" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>00.10.1998</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>6</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>14</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>9</v>
+      </c>
+      <c r="M8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>00.10.42</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>14</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>9</v>
+      </c>
+      <c r="M9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>03.05.1979</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>14</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>9</v>
+      </c>
+      <c r="M10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>03.05.1979</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>55NM123</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>14</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Nisa Karaman</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2357</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2578</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>853</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2368</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>4680</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>3568</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>169</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>9643</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>3827</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Sgkhfbll</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>588</v>
+      </c>
+      <c r="M12" t="n">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>15.02.2025</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>68HS574</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>14</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Melih Karaman</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>9</v>
+      </c>
+      <c r="M13" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>11.07.2025</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>45HD132</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>564</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>614</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>617</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>50</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ela karaman </t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>116</v>
+      </c>
+      <c r="M14" t="n">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>